<commit_message>
Simplified and fixed any issues inside leave request modal!
</commit_message>
<xml_diff>
--- a/public/inventory_details.xlsx
+++ b/public/inventory_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisj\OneDrive\Documents\HQ-App\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F6EF65-E295-4F1F-948A-5CB14BBBFC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182CF905-1B6B-4BF7-BCA4-63D17D166692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5438" uniqueCount="1751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5439" uniqueCount="1752">
   <si>
     <t>IT Room</t>
   </si>
@@ -5365,6 +5365,9 @@
   </si>
   <si>
     <t>Description2</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -6264,7 +6267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A639" zoomScale="56" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H682" sqref="H682"/>
     </sheetView>
   </sheetViews>
@@ -23631,67 +23634,70 @@
       <c r="C672" s="14"/>
       <c r="D672" s="14"/>
     </row>
-    <row r="673" spans="3:4">
+    <row r="673" spans="3:8">
       <c r="C673" s="14"/>
       <c r="D673" s="14"/>
     </row>
-    <row r="674" spans="3:4">
+    <row r="674" spans="3:8">
       <c r="C674" s="14"/>
       <c r="D674" s="14"/>
     </row>
-    <row r="675" spans="3:4">
+    <row r="675" spans="3:8">
       <c r="C675" s="14"/>
       <c r="D675" s="14"/>
     </row>
-    <row r="676" spans="3:4">
+    <row r="676" spans="3:8">
       <c r="C676" s="14"/>
       <c r="D676" s="14"/>
     </row>
-    <row r="677" spans="3:4">
+    <row r="677" spans="3:8">
       <c r="C677" s="14"/>
       <c r="D677" s="14"/>
     </row>
-    <row r="678" spans="3:4">
+    <row r="678" spans="3:8">
       <c r="C678" s="14"/>
       <c r="D678" s="14"/>
     </row>
-    <row r="679" spans="3:4">
+    <row r="679" spans="3:8">
       <c r="C679" s="14"/>
       <c r="D679" s="14"/>
     </row>
-    <row r="680" spans="3:4">
+    <row r="680" spans="3:8">
       <c r="C680" s="14"/>
       <c r="D680" s="14"/>
     </row>
-    <row r="681" spans="3:4">
+    <row r="681" spans="3:8">
       <c r="C681" s="14"/>
       <c r="D681" s="14"/>
     </row>
-    <row r="682" spans="3:4">
+    <row r="682" spans="3:8">
       <c r="C682" s="14"/>
       <c r="D682" s="14"/>
-    </row>
-    <row r="683" spans="3:4">
+      <c r="H682" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="683" spans="3:8">
       <c r="C683" s="14"/>
       <c r="D683" s="14"/>
     </row>
-    <row r="684" spans="3:4">
+    <row r="684" spans="3:8">
       <c r="C684" s="14"/>
       <c r="D684" s="14"/>
     </row>
-    <row r="685" spans="3:4">
+    <row r="685" spans="3:8">
       <c r="C685" s="14"/>
       <c r="D685" s="14"/>
     </row>
-    <row r="686" spans="3:4">
+    <row r="686" spans="3:8">
       <c r="C686" s="14"/>
       <c r="D686" s="14"/>
     </row>
-    <row r="687" spans="3:4">
+    <row r="687" spans="3:8">
       <c r="C687" s="14"/>
       <c r="D687" s="14"/>
     </row>
-    <row r="688" spans="3:4">
+    <row r="688" spans="3:8">
       <c r="C688" s="14"/>
       <c r="D688" s="14"/>
     </row>

</xml_diff>